<commit_message>
some pcb errors are labeled
</commit_message>
<xml_diff>
--- a/pcb/pinout.xlsx
+++ b/pcb/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\onlab\Digital_guitar_effect\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aron\Documents\GitHub\Digital_guitar_effect\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033C7D22-1F24-48ED-B3F3-375D48ABB174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389FE738-31D9-4DE4-81D6-1A6366061BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22908" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1ECC89A-70EF-4060-9F61-ECE5038C6326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,12 +371,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -386,28 +401,28 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -727,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFBBC6E-FF7A-4C12-8012-F4C4CA447A76}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A34"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,48 +756,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F4">
@@ -791,354 +808,356 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" t="s">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C37">
         <f>+COUNTA(C2:C34)</f>
         <v>33</v>

</xml_diff>